<commit_message>
I had a Canadian friend look things over, he suggested some thing we missed.
</commit_message>
<xml_diff>
--- a/Stability Coding.xlsx
+++ b/Stability Coding.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4540" yWindow="460" windowWidth="16220" windowHeight="16420" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="4540" yWindow="460" windowWidth="16220" windowHeight="16420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="General" sheetId="4" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3847" uniqueCount="3572">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3855" uniqueCount="3580">
   <si>
     <t>Mounties</t>
   </si>
@@ -10830,19 +10830,36 @@
       <t>;</t>
     </r>
   </si>
+  <si>
+    <t>religious freedom</t>
+  </si>
+  <si>
+    <t>liberté de religion</t>
+  </si>
+  <si>
+    <t>uhuru wa dini</t>
+  </si>
+  <si>
+    <t>subsidy</t>
+  </si>
+  <si>
+    <t>ruzuku</t>
+  </si>
+  <si>
+    <t>subvention</t>
+  </si>
+  <si>
+    <t>subventionné</t>
+  </si>
+  <si>
+    <t>subsidized</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -10942,30 +10959,30 @@
   </borders>
   <cellStyleXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -11270,10 +11287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C238"/>
+  <dimension ref="A1:C241"/>
   <sheetViews>
-    <sheetView topLeftCell="A231" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A231" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="160" workbookViewId="0">
+      <selection activeCell="A246" sqref="A246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13668,6 +13685,36 @@
         <v>3555</v>
       </c>
     </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A239" s="3" t="s">
+        <v>3572</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>3574</v>
+      </c>
+      <c r="C239" s="5" t="s">
+        <v>3573</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A240" s="3" t="s">
+        <v>3575</v>
+      </c>
+      <c r="B240" s="3" t="s">
+        <v>3576</v>
+      </c>
+      <c r="C240" s="5" t="s">
+        <v>3577</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A241" s="3" t="s">
+        <v>3579</v>
+      </c>
+      <c r="C241" s="5" t="s">
+        <v>3578</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13677,7 +13724,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F1303"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
+    <sheetView topLeftCell="A126" zoomScale="170" zoomScaleNormal="170" zoomScalePageLayoutView="170" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>